<commit_message>
Remove legacy scripts and batch files for profile management and scraping
- Deleted `ajouter_profils.bat` and `ajouter_profils.py` as they are no longer needed.
- Removed `profile_scraper.py` which contained the main scraping logic.
- Eliminated `recherche_anti_captcha.bat` and `recherche_avec_ajout.bat` batch files that facilitated anti-captcha searches and profile additions.
</commit_message>
<xml_diff>
--- a/Resultats_Profils.xlsx
+++ b/Resultats_Profils.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,105 +470,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>développeur Python</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Profil</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Linkedin</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Atos</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>https://fr.linkedin.com/in/julien-millot</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-06-30 14:14:28</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>développeur Python</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Profil</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Linkedin</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Sopra Steria</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>https://fr.linkedin.com/in/florian-bautry</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2025-06-30 14:14:29</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>développeur Python</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Profil</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Linkedin</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Orange Business</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>https://fr.linkedin.com/in/haroldhaldemann</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2025-06-30 14:14:31</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>